<commit_message>
everything is done except some styling
</commit_message>
<xml_diff>
--- a/public/reports/goods_recieving_note_g.xlsx
+++ b/public/reports/goods_recieving_note_g.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>UNIFORMS &amp; TEXTILE MANUFECTURING CO.</t>
   </si>
@@ -36,7 +36,7 @@
     <t>INVOICE No:</t>
   </si>
   <si>
-    <t>8787878</t>
+    <t>34343</t>
   </si>
   <si>
     <t>ADDRESS:</t>
@@ -48,7 +48,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>2019-01-19</t>
+    <t>2019-01-18</t>
   </si>
   <si>
     <t>CONTACT PERSON:</t>
@@ -72,7 +72,7 @@
     <t>Received By</t>
   </si>
   <si>
-    <t>ahmed</t>
+    <t>ALI</t>
   </si>
   <si>
     <t>Received Qty</t>
@@ -90,19 +90,16 @@
     <t>Total Amount PKR</t>
   </si>
   <si>
-    <t>950</t>
+    <t>500</t>
   </si>
   <si>
     <t>cotton-1000</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
-    <t>599</t>
+    <t>299</t>
   </si>
   <si>
     <t>cloth-a-some description</t>
@@ -3960,33 +3957,33 @@
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="24" t="s">
-        <v>26</v>
-      </c>
       <c r="H17" s="25">
-        <v>14250</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="18" ht="20.1" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>27</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>28</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="25">
-        <v>59900</v>
+        <v>29900</v>
       </c>
     </row>
     <row r="19" ht="20.1" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4166,16 +4163,16 @@
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G36" s="26"/>
       <c r="H36" s="25">
-        <v>74150</v>
+        <v>37400</v>
       </c>
     </row>
     <row r="37" ht="15" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -4187,7 +4184,7 @@
     </row>
     <row r="38" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="27"/>
       <c r="C38" s="27"/>
@@ -4195,7 +4192,7 @@
     </row>
     <row r="39" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H39" s="28"/>
     </row>
@@ -4205,20 +4202,20 @@
     </row>
     <row r="41" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="28"/>
     </row>
     <row r="42" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F42" s="33" t="s">
         <v>36</v>
-      </c>
-      <c r="F42" s="33" t="s">
-        <v>37</v>
       </c>
       <c r="G42" s="33"/>
       <c r="H42" s="28"/>
@@ -4231,20 +4228,20 @@
     </row>
     <row r="45" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H45" s="28"/>
     </row>
     <row r="46" ht="15" customHeight="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H46" s="28"/>
     </row>
     <row r="47" ht="15" customHeight="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" s="34"/>
       <c r="C47" s="34"/>
@@ -4257,7 +4254,7 @@
     </row>
     <row r="48" ht="15" customHeight="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" s="36"/>
       <c r="C48" s="36"/>
@@ -4270,7 +4267,7 @@
     </row>
     <row r="49" ht="15" customHeight="1" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B49" s="37"/>
       <c r="C49" s="37"/>

</xml_diff>